<commit_message>
added full NM to data files
</commit_message>
<xml_diff>
--- a/NMxAccuracy/data/NMxPositiveAccuracy_anova.xlsx
+++ b/NMxAccuracy/data/NMxPositiveAccuracy_anova.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tun46412/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/NMxAccuracy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8AECF-6297-1A4D-885E-35F808954D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46786C43-6E79-F945-BB68-31EE14405819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3660" windowWidth="16820" windowHeight="15620" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
+    <workbookView xWindow="4680" yWindow="460" windowWidth="16820" windowHeight="14780" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,9 +39,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>NM</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -178,6 +184,9 @@
   </si>
   <si>
     <t>SVS</t>
+  </si>
+  <si>
+    <t>NM_vstri</t>
   </si>
 </sst>
 </file>
@@ -640,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31723B7A-45ED-944A-9BE0-99732653F64A}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M71" sqref="M71:P71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,54 +660,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5">
         <v>6.6323999999999996</v>
@@ -752,7 +761,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>5.8707000000000003</v>
@@ -806,7 +815,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>10.6219</v>
@@ -860,7 +869,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>6.7069999999999999</v>
@@ -914,7 +923,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>9.8196999999999992</v>
@@ -968,7 +977,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>9.8634000000000004</v>
@@ -1022,7 +1031,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>6.4911000000000003</v>
@@ -1076,7 +1085,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5">
         <v>3.8052999999999999</v>
@@ -1130,7 +1139,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
         <v>8.9419000000000004</v>
@@ -1184,7 +1193,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5">
         <v>7.8029000000000002</v>
@@ -1238,7 +1247,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5">
         <v>9.8434000000000008</v>
@@ -1292,7 +1301,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5">
         <v>6.5369000000000002</v>
@@ -1346,7 +1355,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5">
         <v>6.3827999999999996</v>
@@ -1400,7 +1409,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5">
         <v>7.1338999999999997</v>
@@ -1454,7 +1463,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5">
         <v>9.2367000000000008</v>
@@ -1508,7 +1517,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5">
         <v>7.0613999999999999</v>
@@ -1562,7 +1571,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5">
         <v>6.7188999999999997</v>
@@ -1616,7 +1625,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5">
         <v>9.7673000000000005</v>
@@ -1670,7 +1679,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5">
         <v>8.6026000000000007</v>
@@ -1724,7 +1733,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5">
         <v>7.6535000000000002</v>
@@ -1778,7 +1787,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5">
         <v>7.0533000000000001</v>
@@ -1832,7 +1841,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5">
         <v>5.4255000000000004</v>
@@ -1886,7 +1895,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="5">
         <v>7.1264000000000003</v>
@@ -1940,7 +1949,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5">
         <v>8.3969000000000005</v>
@@ -1994,7 +2003,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5">
         <v>10.875999999999999</v>
@@ -2048,7 +2057,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5">
         <v>8.4403000000000006</v>
@@ -2102,7 +2111,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5">
         <v>6.7473000000000001</v>
@@ -2156,7 +2165,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5">
         <v>5.7484999999999999</v>
@@ -2210,7 +2219,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5">
         <v>6.6740000000000004</v>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5">
         <v>7.1413000000000002</v>
@@ -2318,7 +2327,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5">
         <v>5.1193</v>
@@ -2372,7 +2381,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5">
         <v>6.8760000000000003</v>
@@ -2426,7 +2435,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5">
         <v>10.682600000000001</v>
@@ -2480,7 +2489,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5">
         <v>9.7484000000000002</v>
@@ -2534,7 +2543,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="5">
         <v>6.3623000000000003</v>
@@ -2588,7 +2597,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" s="5">
         <v>6.6323999999999996</v>
@@ -2642,7 +2651,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="5">
         <v>5.8707000000000003</v>
@@ -2696,7 +2705,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" s="5">
         <v>10.6219</v>
@@ -2750,7 +2759,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="5">
         <v>6.7069999999999999</v>
@@ -2804,7 +2813,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" s="5">
         <v>9.8196999999999992</v>
@@ -2858,7 +2867,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="5">
         <v>9.8634000000000004</v>
@@ -2912,7 +2921,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="5">
         <v>6.4911000000000003</v>
@@ -2966,7 +2975,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="5">
         <v>3.8052999999999999</v>
@@ -3020,7 +3029,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="5">
         <v>8.9419000000000004</v>
@@ -3074,7 +3083,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="5">
         <v>7.8029000000000002</v>
@@ -3128,7 +3137,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" s="5">
         <v>9.8434000000000008</v>
@@ -3182,7 +3191,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" s="5">
         <v>6.5369000000000002</v>
@@ -3236,7 +3245,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" s="5">
         <v>6.3827999999999996</v>
@@ -3290,7 +3299,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" s="5">
         <v>7.1338999999999997</v>
@@ -3344,7 +3353,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" s="5">
         <v>9.2367000000000008</v>
@@ -3398,7 +3407,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B52" s="5">
         <v>7.0613999999999999</v>
@@ -3452,7 +3461,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="5">
         <v>6.7188999999999997</v>
@@ -3506,7 +3515,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="5">
         <v>9.7673000000000005</v>
@@ -3560,7 +3569,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B55" s="5">
         <v>8.6026000000000007</v>
@@ -3614,7 +3623,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B56" s="5">
         <v>7.6535000000000002</v>
@@ -3668,7 +3677,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" s="5">
         <v>7.0533000000000001</v>
@@ -3722,7 +3731,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="5">
         <v>5.4255000000000004</v>
@@ -3776,7 +3785,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="5">
         <v>7.1264000000000003</v>
@@ -3830,7 +3839,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="5">
         <v>8.3969000000000005</v>
@@ -3884,7 +3893,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61" s="5">
         <v>10.875999999999999</v>
@@ -3938,7 +3947,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B62" s="5">
         <v>8.4403000000000006</v>
@@ -3992,7 +4001,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B63" s="5">
         <v>6.7473000000000001</v>
@@ -4046,7 +4055,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" s="5">
         <v>5.7484999999999999</v>
@@ -4100,7 +4109,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B65" s="5">
         <v>6.6740000000000004</v>
@@ -4154,7 +4163,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B66" s="5">
         <v>7.1413000000000002</v>
@@ -4208,7 +4217,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67" s="5">
         <v>5.1193</v>
@@ -4262,7 +4271,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68" s="5">
         <v>6.8760000000000003</v>
@@ -4316,7 +4325,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69" s="5">
         <v>10.682600000000001</v>
@@ -4370,7 +4379,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70" s="5">
         <v>9.7484000000000002</v>
@@ -4424,7 +4433,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" s="8">
         <v>6.3623000000000003</v>

</xml_diff>

<commit_message>
update nm full plots
</commit_message>
<xml_diff>
--- a/NMxAccuracy/data/NMxPositiveAccuracy_anova.xlsx
+++ b/NMxAccuracy/data/NMxPositiveAccuracy_anova.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/NMxAccuracy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46786C43-6E79-F945-BB68-31EE14405819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64CF576-E3CA-2E45-9368-CC631B333002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="460" windowWidth="16820" windowHeight="14780" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
+    <workbookView xWindow="4680" yWindow="460" windowWidth="16820" windowHeight="14760" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
     <t>SVS</t>
   </si>
   <si>
-    <t>NM_vstri</t>
+    <t>NM</t>
   </si>
 </sst>
 </file>

</xml_diff>